<commit_message>
Worked on #2 - Added col_helpers.R - Generalized get_stat_per_day() - Added Debug functionality - Added extra columns to translation key
</commit_message>
<xml_diff>
--- a/translation_key.xlsx
+++ b/translation_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skirsch\Desktop\Projects\CNP m-Path-fitbit data tidying\m-Path\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skirsch\surfdrive\Projects\CNP\CNP m-Path-fitbit data tidying\mpath_fitbit_merge_and_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CCE0B772-9D77-4C17-85E3-A62C2A6226DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84A0F57-5BFA-4EB2-BD96-9FCFABEDE203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37875" yWindow="1305" windowWidth="13665" windowHeight="14370"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation_key" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="154">
   <si>
     <t>Asleep</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Pain</t>
   </si>
   <si>
-    <t>Pijn_waar (bodyParts)</t>
-  </si>
-  <si>
     <t>Pain_where</t>
   </si>
   <si>
@@ -470,12 +467,27 @@
   </si>
   <si>
     <t>Medication</t>
+  </si>
+  <si>
+    <t>Pijn_waar</t>
+  </si>
+  <si>
+    <t>Medicatie_inhoud (open)</t>
+  </si>
+  <si>
+    <t>Medication_content</t>
+  </si>
+  <si>
+    <t>start_vragenlijsten_week</t>
+  </si>
+  <si>
+    <t>Start_questionnaire_week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1310,11 +1322,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,18 +1337,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1347,7 +1359,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1358,7 +1370,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1369,7 +1381,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1380,7 +1392,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1391,7 +1403,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1402,7 +1414,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1413,7 +1425,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -1424,7 +1436,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1435,7 +1447,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1446,7 +1458,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -1457,7 +1469,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -1468,7 +1480,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -1479,7 +1491,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -1501,7 +1513,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -1512,7 +1524,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1523,7 +1535,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1534,7 +1546,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1545,10 +1557,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1556,10 +1568,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1567,10 +1579,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1578,21 +1590,21 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
         <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -1600,10 +1612,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1611,10 +1623,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1622,10 +1634,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -1633,10 +1645,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
       </c>
       <c r="C29" t="b">
         <v>1</v>
@@ -1644,10 +1656,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
@@ -1655,10 +1667,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
@@ -1666,10 +1678,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
@@ -1677,10 +1689,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="b">
         <v>1</v>
@@ -1688,10 +1700,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
@@ -1699,10 +1711,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
@@ -1710,10 +1722,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
@@ -1721,10 +1733,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
@@ -1732,10 +1744,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="b">
         <v>1</v>
@@ -1743,21 +1755,21 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
@@ -1765,10 +1777,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
@@ -1776,10 +1788,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" t="b">
         <v>1</v>
@@ -1787,10 +1799,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
@@ -1798,10 +1810,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
@@ -1809,10 +1821,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
         <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>47</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -1820,10 +1832,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -1831,10 +1843,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
@@ -1842,10 +1854,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -1853,10 +1865,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
         <v>50</v>
-      </c>
-      <c r="B49" t="s">
-        <v>51</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
@@ -1864,10 +1876,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
@@ -1875,10 +1887,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -1886,10 +1898,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -1897,10 +1909,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -1908,10 +1920,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" t="b">
         <v>1</v>
@@ -1919,10 +1931,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -1930,10 +1942,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
@@ -1941,10 +1953,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
@@ -1952,10 +1964,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -1963,10 +1975,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -1974,10 +1986,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
@@ -1985,10 +1997,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
@@ -1996,10 +2008,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -2007,10 +2019,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63" t="b">
         <v>1</v>
@@ -2018,10 +2030,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
@@ -2029,10 +2041,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -2040,10 +2052,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -2051,10 +2063,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -2062,10 +2074,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -2073,10 +2085,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -2084,21 +2096,21 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" t="b">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="C70" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -2106,10 +2118,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -2117,10 +2129,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -2128,10 +2140,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -2139,13 +2151,35 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated readme and translation_key.xslx closes #7
</commit_message>
<xml_diff>
--- a/translation_key.xlsx
+++ b/translation_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skirsch\surfdrive\Projects\CNP\CNP m-Path-fitbit data tidying\mpath_fitbit_merge_and_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84A0F57-5BFA-4EB2-BD96-9FCFABEDE203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0302F9-A749-4AB1-91D2-E7B8E2123F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="1380" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translation_key" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="155">
   <si>
     <t>Asleep</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>Start_questionnaire_week</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -965,9 +968,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1323,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,22 +1351,22 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1370,10 +1374,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -1381,10 +1385,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -1392,10 +1396,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -1403,10 +1407,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -1414,10 +1418,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -1425,10 +1429,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -1436,10 +1440,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -1447,10 +1451,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1458,10 +1462,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1469,10 +1473,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -1480,10 +1484,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1491,10 +1495,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1502,10 +1506,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1513,10 +1517,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1524,10 +1528,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1535,10 +1539,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1546,10 +1550,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1557,10 +1561,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1568,10 +1572,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1579,10 +1583,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1590,32 +1594,32 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1623,10 +1627,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1634,10 +1638,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -1645,10 +1649,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" t="b">
         <v>1</v>
@@ -1656,10 +1660,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
@@ -1667,10 +1671,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
@@ -1678,10 +1682,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
@@ -1689,10 +1693,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="b">
         <v>1</v>
@@ -1700,10 +1704,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
@@ -1711,10 +1715,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
@@ -1722,10 +1726,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
@@ -1733,10 +1737,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
@@ -1744,10 +1748,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" t="b">
         <v>1</v>
@@ -1755,32 +1759,32 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" t="b">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
@@ -1788,10 +1792,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" t="b">
         <v>1</v>
@@ -1799,10 +1803,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
@@ -1810,10 +1814,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
@@ -1821,10 +1825,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -1832,10 +1836,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -1843,10 +1847,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
@@ -1854,10 +1858,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -1865,10 +1869,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
@@ -1876,10 +1880,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
@@ -1887,10 +1891,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -1898,10 +1902,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -1909,10 +1913,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -1920,10 +1924,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" t="b">
         <v>1</v>
@@ -1931,10 +1935,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -1942,10 +1946,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
@@ -1953,10 +1957,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
@@ -1964,10 +1968,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -1975,10 +1979,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -1986,10 +1990,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
@@ -1997,10 +2001,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
@@ -2008,10 +2012,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -2019,10 +2023,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C63" t="b">
         <v>1</v>
@@ -2030,10 +2034,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
@@ -2041,10 +2045,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -2052,10 +2056,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -2063,10 +2067,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -2074,10 +2078,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -2085,10 +2089,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -2096,32 +2100,32 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
-        <v>151</v>
-      </c>
-      <c r="C70" t="s">
-        <v>23</v>
+        <v>148</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" t="b">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="C71" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -2129,10 +2133,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -2140,10 +2144,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -2151,10 +2155,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -2162,10 +2166,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>
@@ -2173,12 +2177,23 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>152</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>153</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>